<commit_message>
more pdfs , bug stil todo
</commit_message>
<xml_diff>
--- a/tables/base_latency_table.xlsx
+++ b/tables/base_latency_table.xlsx
@@ -522,76 +522,76 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>41.628773</v>
+        <v>41.502507</v>
       </c>
       <c r="C2" t="n">
-        <v>33.954663</v>
+        <v>33.943337</v>
       </c>
       <c r="D2" t="n">
-        <v>33.4087575</v>
+        <v>33.4099445</v>
       </c>
       <c r="E2" t="n">
-        <v>33.3004845</v>
+        <v>33.283971</v>
       </c>
       <c r="F2" t="n">
-        <v>33.1292515</v>
+        <v>33.1262525</v>
       </c>
       <c r="G2" t="n">
-        <v>32.932178</v>
+        <v>32.935083</v>
       </c>
       <c r="H2" t="n">
-        <v>32.787051</v>
+        <v>32.804916</v>
       </c>
       <c r="I2" t="n">
-        <v>32.5981405</v>
+        <v>32.6085545</v>
       </c>
       <c r="J2" t="n">
-        <v>32.5021485</v>
+        <v>32.5112955</v>
       </c>
       <c r="K2" t="n">
-        <v>32.433976</v>
+        <v>32.409966</v>
       </c>
       <c r="L2" t="n">
-        <v>32.224368</v>
+        <v>32.2237045</v>
       </c>
       <c r="M2" t="n">
-        <v>32.15160299999999</v>
+        <v>32.163314</v>
       </c>
       <c r="N2" t="n">
-        <v>32.038974</v>
+        <v>32.045982</v>
       </c>
       <c r="O2" t="n">
-        <v>31.985102</v>
+        <v>32.001113</v>
       </c>
       <c r="P2" t="n">
-        <v>31.965719</v>
+        <v>31.9845</v>
       </c>
       <c r="Q2" t="n">
-        <v>31.916407</v>
+        <v>31.923474</v>
       </c>
       <c r="R2" t="n">
-        <v>31.916791</v>
+        <v>31.9156455</v>
       </c>
       <c r="S2" t="n">
-        <v>31.8291145</v>
+        <v>31.824707</v>
       </c>
       <c r="T2" t="n">
-        <v>31.855958</v>
+        <v>31.848388</v>
       </c>
       <c r="U2" t="n">
-        <v>31.826632</v>
+        <v>31.8285285</v>
       </c>
       <c r="V2" t="n">
-        <v>31.834164</v>
+        <v>31.830361</v>
       </c>
       <c r="W2" t="n">
-        <v>31.952834</v>
+        <v>31.964609</v>
       </c>
       <c r="X2" t="n">
-        <v>32.29776649999999</v>
+        <v>32.264929</v>
       </c>
       <c r="Y2" t="n">
-        <v>32.7193585</v>
+        <v>32.1692005</v>
       </c>
       <c r="Z2" t="n">
         <v>31.780215</v>
@@ -607,73 +607,73 @@
         <v>21.778655</v>
       </c>
       <c r="C3" t="n">
-        <v>18.420343</v>
+        <v>18.415742</v>
       </c>
       <c r="D3" t="n">
-        <v>17.961621</v>
+        <v>17.990936</v>
       </c>
       <c r="E3" t="n">
-        <v>18.002242</v>
+        <v>18.021751</v>
       </c>
       <c r="F3" t="n">
-        <v>18.0002745</v>
+        <v>18.0168695</v>
       </c>
       <c r="G3" t="n">
-        <v>17.9348105</v>
+        <v>17.971869</v>
       </c>
       <c r="H3" t="n">
-        <v>17.944798</v>
+        <v>17.972097</v>
       </c>
       <c r="I3" t="n">
-        <v>18.070119</v>
+        <v>18.106831</v>
       </c>
       <c r="J3" t="n">
-        <v>18.245024</v>
+        <v>18.31331</v>
       </c>
       <c r="K3" t="n">
-        <v>18.055884</v>
+        <v>18.07888</v>
       </c>
       <c r="L3" t="n">
-        <v>17.852205</v>
+        <v>17.866344</v>
       </c>
       <c r="M3" t="n">
-        <v>17.8877855</v>
+        <v>17.918727</v>
       </c>
       <c r="N3" t="n">
-        <v>18.063787</v>
+        <v>18.091247</v>
       </c>
       <c r="O3" t="n">
-        <v>18.46324</v>
+        <v>18.502851</v>
       </c>
       <c r="P3" t="n">
-        <v>18.091081</v>
+        <v>18.1294</v>
       </c>
       <c r="Q3" t="n">
-        <v>17.799368</v>
+        <v>17.817797</v>
       </c>
       <c r="R3" t="n">
-        <v>17.756512</v>
+        <v>17.7911055</v>
       </c>
       <c r="S3" t="n">
-        <v>17.663547</v>
+        <v>17.690076</v>
       </c>
       <c r="T3" t="n">
-        <v>17.6158865</v>
+        <v>17.648954</v>
       </c>
       <c r="U3" t="n">
-        <v>17.555709</v>
+        <v>17.59945</v>
       </c>
       <c r="V3" t="n">
-        <v>17.567527</v>
+        <v>17.596235</v>
       </c>
       <c r="W3" t="n">
-        <v>17.569635</v>
+        <v>17.6140005</v>
       </c>
       <c r="X3" t="n">
-        <v>17.540994</v>
+        <v>17.6011135</v>
       </c>
       <c r="Y3" t="n">
-        <v>17.025486</v>
+        <v>17.107424</v>
       </c>
       <c r="Z3" t="inlineStr"/>
     </row>
@@ -684,73 +684,73 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1034.041348</v>
+        <v>1049.770767</v>
       </c>
       <c r="C4" t="n">
-        <v>648.2423725</v>
+        <v>681.5901995</v>
       </c>
       <c r="D4" t="n">
-        <v>40.950913</v>
+        <v>41.091653</v>
       </c>
       <c r="E4" t="n">
-        <v>40.558868</v>
+        <v>40.576664</v>
       </c>
       <c r="F4" t="n">
-        <v>40.492594</v>
+        <v>40.505575</v>
       </c>
       <c r="G4" t="n">
-        <v>40.457233</v>
+        <v>40.466164</v>
       </c>
       <c r="H4" t="n">
-        <v>40.437237</v>
+        <v>40.442342</v>
       </c>
       <c r="I4" t="n">
-        <v>40.413307</v>
+        <v>40.41662</v>
       </c>
       <c r="J4" t="n">
-        <v>40.365685</v>
+        <v>40.377234</v>
       </c>
       <c r="K4" t="n">
-        <v>40.3570275</v>
+        <v>40.368282</v>
       </c>
       <c r="L4" t="n">
-        <v>40.3251075</v>
+        <v>40.333146</v>
       </c>
       <c r="M4" t="n">
-        <v>40.368451</v>
+        <v>40.374788</v>
       </c>
       <c r="N4" t="n">
-        <v>40.3594975</v>
+        <v>40.3647485</v>
       </c>
       <c r="O4" t="n">
-        <v>40.359018</v>
+        <v>40.362897</v>
       </c>
       <c r="P4" t="n">
-        <v>40.341914</v>
+        <v>40.34608</v>
       </c>
       <c r="Q4" t="n">
-        <v>40.3312745</v>
+        <v>40.338186</v>
       </c>
       <c r="R4" t="n">
-        <v>40.328869</v>
+        <v>40.338728</v>
       </c>
       <c r="S4" t="n">
-        <v>40.342489</v>
+        <v>40.3578675</v>
       </c>
       <c r="T4" t="n">
-        <v>40.31189</v>
+        <v>40.329247</v>
       </c>
       <c r="U4" t="n">
-        <v>40.323129</v>
+        <v>40.333388</v>
       </c>
       <c r="V4" t="n">
-        <v>40.3183645</v>
+        <v>40.3309715</v>
       </c>
       <c r="W4" t="n">
-        <v>40.3840465</v>
+        <v>40.399623</v>
       </c>
       <c r="X4" t="n">
-        <v>40.481896</v>
+        <v>40.487854</v>
       </c>
       <c r="Y4" t="n">
         <v>40.667081</v>
@@ -766,76 +766,76 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>438.579502</v>
+        <v>443.147291</v>
       </c>
       <c r="C5" t="n">
-        <v>65.9548175</v>
+        <v>65.955372</v>
       </c>
       <c r="D5" t="n">
-        <v>41.8283445</v>
+        <v>41.767088</v>
       </c>
       <c r="E5" t="n">
-        <v>41.387153</v>
+        <v>41.3594285</v>
       </c>
       <c r="F5" t="n">
-        <v>41.185464</v>
+        <v>41.159949</v>
       </c>
       <c r="G5" t="n">
-        <v>40.9473835</v>
+        <v>40.92487850000001</v>
       </c>
       <c r="H5" t="n">
-        <v>40.8396</v>
+        <v>40.825615</v>
       </c>
       <c r="I5" t="n">
-        <v>40.8063145</v>
+        <v>40.7838535</v>
       </c>
       <c r="J5" t="n">
-        <v>40.760926</v>
+        <v>40.739068</v>
       </c>
       <c r="K5" t="n">
-        <v>40.73137</v>
+        <v>40.713392</v>
       </c>
       <c r="L5" t="n">
-        <v>40.721935</v>
+        <v>40.691439</v>
       </c>
       <c r="M5" t="n">
-        <v>40.6852215</v>
+        <v>40.667528</v>
       </c>
       <c r="N5" t="n">
-        <v>40.684442</v>
+        <v>40.6767145</v>
       </c>
       <c r="O5" t="n">
-        <v>40.668002</v>
+        <v>40.658665</v>
       </c>
       <c r="P5" t="n">
-        <v>40.78399</v>
+        <v>40.7646015</v>
       </c>
       <c r="Q5" t="n">
-        <v>41.01182</v>
+        <v>40.994513</v>
       </c>
       <c r="R5" t="n">
-        <v>41.29573</v>
+        <v>41.282023</v>
       </c>
       <c r="S5" t="n">
-        <v>41.555743</v>
+        <v>41.525326</v>
       </c>
       <c r="T5" t="n">
-        <v>41.678376</v>
+        <v>41.632725</v>
       </c>
       <c r="U5" t="n">
-        <v>41.633659</v>
+        <v>41.60699</v>
       </c>
       <c r="V5" t="n">
-        <v>41.171377</v>
+        <v>41.1323295</v>
       </c>
       <c r="W5" t="n">
-        <v>40.635036</v>
+        <v>40.637392</v>
       </c>
       <c r="X5" t="n">
         <v>40.64081</v>
       </c>
       <c r="Y5" t="n">
-        <v>42.7694555</v>
+        <v>42.758387</v>
       </c>
       <c r="Z5" t="n">
         <v>51.1010335</v>

</xml_diff>